<commit_message>
some new files and code edits
</commit_message>
<xml_diff>
--- a/excelpractice/book2.xlsx
+++ b/excelpractice/book2.xlsx
@@ -1,66 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>mercury</t>
-  </si>
-  <si>
-    <t>sga</t>
-  </si>
-  <si>
-    <t>uhhuh</t>
-  </si>
-  <si>
-    <t>ggdjkgda</t>
-  </si>
-  <si>
-    <t>ghggjh</t>
-  </si>
-  <si>
-    <t>gfhjgf</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,14 +54,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,87 +416,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="11.7109375" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mercury</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mercury</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mercury</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sga</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>uhhuh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ggdjkgda</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>gfhjgf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ghggjh</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>